<commit_message>
update LWC package and TB
</commit_message>
<xml_diff>
--- a/doc/sparkle.xlsx
+++ b/doc/sparkle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamyar/src/sparkle/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5747B96A-349E-6D43-81A8-FED708C61892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD509D-4DE8-8047-AF99-2B733BFFB97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="500" windowWidth="39320" windowHeight="24700" xr2:uid="{184C1FB9-41F6-024C-85C4-C8181ECF4CD3}"/>
+    <workbookView xWindow="2140" yWindow="500" windowWidth="41240" windowHeight="24700" xr2:uid="{184C1FB9-41F6-024C-85C4-C8181ECF4CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix issue with stalls, update LWC pkg
</commit_message>
<xml_diff>
--- a/doc/sparkle.xlsx
+++ b/doc/sparkle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamyar/src/sparkle/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD509D-4DE8-8047-AF99-2B733BFFB97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D12D2D-CD66-C140-9FB2-F7DBB74C39E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="500" windowWidth="41240" windowHeight="24700" xr2:uid="{184C1FB9-41F6-024C-85C4-C8181ECF4CD3}"/>
+    <workbookView xWindow="49320" yWindow="2760" windowWidth="41240" windowHeight="24700" xr2:uid="{184C1FB9-41F6-024C-85C4-C8181ECF4CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="237" zoomScaleNormal="237" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,21 +481,21 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>2297</v>
+        <v>2246</v>
       </c>
       <c r="D2">
-        <v>1282</v>
+        <v>1261</v>
       </c>
       <c r="E2">
         <v>2129</v>
       </c>
       <c r="F2">
         <f>C2-E2</f>
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="G2">
-        <f>95</f>
-        <v>95</v>
+        <f>98</f>
+        <v>98</v>
       </c>
       <c r="H2">
         <f>8</f>
@@ -503,25 +503,25 @@
       </c>
       <c r="I2" s="2">
         <f>G2/H2</f>
-        <v>11.875</v>
+        <v>12.25</v>
       </c>
       <c r="J2" s="2">
         <f>I2*256</f>
-        <v>3040</v>
+        <v>3136</v>
       </c>
       <c r="K2" s="2">
         <f>I2/I4</f>
-        <v>4.1342592592592595</v>
+        <v>4.2648148148148151</v>
       </c>
       <c r="L2">
         <f>C4/C2</f>
-        <v>1.3369612538093165</v>
+        <v>1.3673196794300979</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>C3/C2</f>
-        <v>1.0487592511972137</v>
+        <v>1.0725734639358859</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -556,7 +556,7 @@
       </c>
       <c r="K3" s="2">
         <f>I3/I2</f>
-        <v>1.1157894736842104</v>
+        <v>1.0816326530612246</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>